<commit_message>
Har færdiggjort de 5 bedste ligaer
</commit_message>
<xml_diff>
--- a/English Premier League/Raw/25_26.xlsx
+++ b/English Premier League/Raw/25_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP17"/>
+  <dimension ref="A1:AP31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2312,22 +2312,22 @@
         <v>8</v>
       </c>
       <c r="J14" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14" t="n">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="L14" t="n">
         <v>12</v>
       </c>
       <c r="M14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O14" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P14" t="n">
         <v>2</v>
@@ -2339,13 +2339,13 @@
         <v>24</v>
       </c>
       <c r="S14" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="T14" t="n">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="U14" t="n">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="V14" t="n">
         <v>82.09999999999999</v>
@@ -2377,19 +2377,19 @@
         <v>17</v>
       </c>
       <c r="AE14" t="n">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="AF14" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AG14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AH14" t="n">
         <v>25</v>
       </c>
       <c r="AI14" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AJ14" t="n">
         <v>2</v>
@@ -2401,16 +2401,16 @@
         <v>18</v>
       </c>
       <c r="AM14" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AN14" t="n">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="AO14" t="n">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="AP14" t="n">
-        <v>71.8</v>
+        <v>71.59999999999999</v>
       </c>
     </row>
     <row r="15">
@@ -2451,19 +2451,19 @@
         <v>11</v>
       </c>
       <c r="K15" t="n">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="L15" t="n">
         <v>28</v>
       </c>
       <c r="M15" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N15" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O15" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P15" t="n">
         <v>1</v>
@@ -2478,13 +2478,13 @@
         <v>59</v>
       </c>
       <c r="T15" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="U15" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="V15" t="n">
-        <v>66.2</v>
+        <v>67.3</v>
       </c>
       <c r="W15" t="inlineStr">
         <is>
@@ -2510,19 +2510,19 @@
         <v>9</v>
       </c>
       <c r="AD15" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE15" t="n">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="AF15" t="n">
         <v>14</v>
       </c>
       <c r="AG15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH15" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AI15" t="n">
         <v>13</v>
@@ -2537,13 +2537,13 @@
         <v>23</v>
       </c>
       <c r="AM15" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AN15" t="n">
-        <v>629</v>
+        <v>642</v>
       </c>
       <c r="AO15" t="n">
-        <v>529</v>
+        <v>540</v>
       </c>
       <c r="AP15" t="n">
         <v>84.09999999999999</v>
@@ -2587,19 +2587,19 @@
         <v>15</v>
       </c>
       <c r="K16" t="n">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="L16" t="n">
         <v>22</v>
       </c>
       <c r="M16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N16" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O16" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
@@ -2608,19 +2608,19 @@
         <v>10</v>
       </c>
       <c r="R16" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S16" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T16" t="n">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="U16" t="n">
         <v>374</v>
       </c>
       <c r="V16" t="n">
-        <v>78.59999999999999</v>
+        <v>78.7</v>
       </c>
       <c r="W16" t="inlineStr">
         <is>
@@ -2649,19 +2649,19 @@
         <v>24</v>
       </c>
       <c r="AE16" t="n">
-        <v>751</v>
+        <v>773</v>
       </c>
       <c r="AF16" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AG16" t="n">
         <v>7</v>
       </c>
       <c r="AH16" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AI16" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AJ16" t="n">
         <v>2</v>
@@ -2670,19 +2670,19 @@
         <v>8</v>
       </c>
       <c r="AL16" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AM16" t="n">
         <v>60</v>
       </c>
       <c r="AN16" t="n">
-        <v>646</v>
+        <v>665</v>
       </c>
       <c r="AO16" t="n">
-        <v>539</v>
+        <v>557</v>
       </c>
       <c r="AP16" t="n">
-        <v>83.40000000000001</v>
+        <v>83.8</v>
       </c>
     </row>
     <row r="17">
@@ -2711,7 +2711,7 @@
         <v>4</v>
       </c>
       <c r="G17" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H17" t="n">
         <v>8</v>
@@ -2723,19 +2723,19 @@
         <v>19</v>
       </c>
       <c r="K17" t="n">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="L17" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M17" t="n">
         <v>5</v>
       </c>
       <c r="N17" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
@@ -2747,16 +2747,16 @@
         <v>28</v>
       </c>
       <c r="S17" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="T17" t="n">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="U17" t="n">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="V17" t="n">
-        <v>90.2</v>
+        <v>90</v>
       </c>
       <c r="W17" t="inlineStr">
         <is>
@@ -2773,7 +2773,7 @@
         <v>1</v>
       </c>
       <c r="AA17" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AB17" t="n">
         <v>11</v>
@@ -2785,10 +2785,10 @@
         <v>5</v>
       </c>
       <c r="AE17" t="n">
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="AF17" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="AG17" t="n">
         <v>6</v>
@@ -2809,16 +2809,1920 @@
         <v>14</v>
       </c>
       <c r="AM17" t="n">
+        <v>44</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>312</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>234</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-08-24</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" t="n">
+        <v>42</v>
+      </c>
+      <c r="H18" t="n">
+        <v>11</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>18</v>
+      </c>
+      <c r="K18" t="n">
+        <v>505</v>
+      </c>
+      <c r="L18" t="n">
+        <v>20</v>
+      </c>
+      <c r="M18" t="n">
+        <v>7</v>
+      </c>
+      <c r="N18" t="n">
+        <v>15</v>
+      </c>
+      <c r="O18" t="n">
+        <v>24</v>
+      </c>
+      <c r="P18" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>11</v>
+      </c>
+      <c r="R18" t="n">
+        <v>14</v>
+      </c>
+      <c r="S18" t="n">
+        <v>59</v>
+      </c>
+      <c r="T18" t="n">
+        <v>413</v>
+      </c>
+      <c r="U18" t="n">
+        <v>307</v>
+      </c>
+      <c r="V18" t="n">
+        <v>74.3</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>Nottingham Forest</t>
+        </is>
+      </c>
+      <c r="X18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>58</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>26</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>665</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>17</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>16</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>16</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>68</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>564</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>462</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>81.90000000000001</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-08-24</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>11</v>
+      </c>
+      <c r="F19" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" t="n">
+        <v>42</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2</v>
+      </c>
+      <c r="J19" t="n">
+        <v>12</v>
+      </c>
+      <c r="K19" t="n">
+        <v>503</v>
+      </c>
+      <c r="L19" t="n">
+        <v>15</v>
+      </c>
+      <c r="M19" t="n">
+        <v>8</v>
+      </c>
+      <c r="N19" t="n">
+        <v>31</v>
+      </c>
+      <c r="O19" t="n">
+        <v>35</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>7</v>
+      </c>
+      <c r="R19" t="n">
+        <v>19</v>
+      </c>
+      <c r="S19" t="n">
+        <v>79</v>
+      </c>
+      <c r="T19" t="n">
+        <v>395</v>
+      </c>
+      <c r="U19" t="n">
+        <v>293</v>
+      </c>
+      <c r="V19" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>Brighton &amp; Hove Albion</t>
+        </is>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>58</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>649</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>17</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>16</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>26</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>27</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>48</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>543</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>449</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>82.7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-08-24</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>13</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" t="n">
+        <v>53</v>
+      </c>
+      <c r="H20" t="n">
+        <v>12</v>
+      </c>
+      <c r="I20" t="n">
+        <v>9</v>
+      </c>
+      <c r="J20" t="n">
+        <v>33</v>
+      </c>
+      <c r="K20" t="n">
+        <v>588</v>
+      </c>
+      <c r="L20" t="n">
+        <v>10</v>
+      </c>
+      <c r="M20" t="n">
+        <v>8</v>
+      </c>
+      <c r="N20" t="n">
+        <v>20</v>
+      </c>
+      <c r="O20" t="n">
+        <v>23</v>
+      </c>
+      <c r="P20" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>9</v>
+      </c>
+      <c r="R20" t="n">
+        <v>21</v>
+      </c>
+      <c r="S20" t="n">
+        <v>60</v>
+      </c>
+      <c r="T20" t="n">
+        <v>479</v>
+      </c>
+      <c r="U20" t="n">
+        <v>386</v>
+      </c>
+      <c r="V20" t="n">
+        <v>80.59999999999999</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>Manchester United</t>
+        </is>
+      </c>
+      <c r="X20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>47</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>553</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>17</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>30</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>17</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>68</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>433</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>348</v>
+      </c>
+      <c r="AP20" t="n">
+        <v>80.40000000000001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Newcastle United</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" t="n">
+        <v>38</v>
+      </c>
+      <c r="H21" t="n">
+        <v>17</v>
+      </c>
+      <c r="I21" t="n">
+        <v>7</v>
+      </c>
+      <c r="J21" t="n">
+        <v>25</v>
+      </c>
+      <c r="K21" t="n">
+        <v>391</v>
+      </c>
+      <c r="L21" t="n">
+        <v>12</v>
+      </c>
+      <c r="M21" t="n">
+        <v>8</v>
+      </c>
+      <c r="N21" t="n">
+        <v>16</v>
+      </c>
+      <c r="O21" t="n">
+        <v>22</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>5</v>
+      </c>
+      <c r="R21" t="n">
+        <v>22</v>
+      </c>
+      <c r="S21" t="n">
+        <v>69</v>
+      </c>
+      <c r="T21" t="n">
+        <v>298</v>
+      </c>
+      <c r="U21" t="n">
+        <v>195</v>
+      </c>
+      <c r="V21" t="n">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="X21" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>62</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>584</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>13</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>17</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>42</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>6</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>19</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>63</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>478</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>390</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>81.59999999999999</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="n">
+        <v>12</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5</v>
+      </c>
+      <c r="G22" t="n">
+        <v>54</v>
+      </c>
+      <c r="H22" t="n">
+        <v>11</v>
+      </c>
+      <c r="I22" t="n">
+        <v>6</v>
+      </c>
+      <c r="J22" t="n">
+        <v>13</v>
+      </c>
+      <c r="K22" t="n">
+        <v>656</v>
+      </c>
+      <c r="L22" t="n">
+        <v>19</v>
+      </c>
+      <c r="M22" t="n">
+        <v>18</v>
+      </c>
+      <c r="N22" t="n">
+        <v>17</v>
+      </c>
+      <c r="O22" t="n">
+        <v>21</v>
+      </c>
+      <c r="P22" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>7</v>
+      </c>
+      <c r="R22" t="n">
+        <v>18</v>
+      </c>
+      <c r="S22" t="n">
+        <v>56</v>
+      </c>
+      <c r="T22" t="n">
+        <v>531</v>
+      </c>
+      <c r="U22" t="n">
+        <v>453</v>
+      </c>
+      <c r="V22" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="X22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="n">
         <v>46</v>
       </c>
-      <c r="AN17" t="n">
+      <c r="AB22" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>15</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>579</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>29</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>13</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>21</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>8</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>75</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>459</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>369</v>
+      </c>
+      <c r="AP22" t="n">
+        <v>80.40000000000001</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Sunderland</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>11</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>54</v>
+      </c>
+      <c r="H23" t="n">
+        <v>11</v>
+      </c>
+      <c r="I23" t="n">
+        <v>3</v>
+      </c>
+      <c r="J23" t="n">
+        <v>18</v>
+      </c>
+      <c r="K23" t="n">
+        <v>574</v>
+      </c>
+      <c r="L23" t="n">
+        <v>28</v>
+      </c>
+      <c r="M23" t="n">
+        <v>7</v>
+      </c>
+      <c r="N23" t="n">
+        <v>23</v>
+      </c>
+      <c r="O23" t="n">
+        <v>35</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>5</v>
+      </c>
+      <c r="R23" t="n">
+        <v>22</v>
+      </c>
+      <c r="S23" t="n">
+        <v>70</v>
+      </c>
+      <c r="T23" t="n">
+        <v>460</v>
+      </c>
+      <c r="U23" t="n">
+        <v>360</v>
+      </c>
+      <c r="V23" t="n">
+        <v>78.3</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="X23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>46</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>510</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>9</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>22</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>34</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>13</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>16</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>61</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>391</v>
+      </c>
+      <c r="AO23" t="n">
         <v>300</v>
       </c>
-      <c r="AO17" t="n">
-        <v>227</v>
-      </c>
-      <c r="AP17" t="n">
-        <v>75.7</v>
+      <c r="AP23" t="n">
+        <v>76.7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Wolverhampton Wanderers</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4</v>
+      </c>
+      <c r="G24" t="n">
+        <v>58</v>
+      </c>
+      <c r="H24" t="n">
+        <v>15</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2</v>
+      </c>
+      <c r="J24" t="n">
+        <v>16</v>
+      </c>
+      <c r="K24" t="n">
+        <v>698</v>
+      </c>
+      <c r="L24" t="n">
+        <v>23</v>
+      </c>
+      <c r="M24" t="n">
+        <v>10</v>
+      </c>
+      <c r="N24" t="n">
+        <v>12</v>
+      </c>
+      <c r="O24" t="n">
+        <v>18</v>
+      </c>
+      <c r="P24" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>4</v>
+      </c>
+      <c r="R24" t="n">
+        <v>30</v>
+      </c>
+      <c r="S24" t="n">
+        <v>76</v>
+      </c>
+      <c r="T24" t="n">
+        <v>576</v>
+      </c>
+      <c r="U24" t="n">
+        <v>461</v>
+      </c>
+      <c r="V24" t="n">
+        <v>80</v>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="X24" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>540</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>16</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>16</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>28</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>78</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>410</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>298</v>
+      </c>
+      <c r="AP24" t="n">
+        <v>72.7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Tottenham Hotspur</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>61</v>
+      </c>
+      <c r="H25" t="n">
+        <v>17</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>20</v>
+      </c>
+      <c r="K25" t="n">
+        <v>671</v>
+      </c>
+      <c r="L25" t="n">
+        <v>16</v>
+      </c>
+      <c r="M25" t="n">
+        <v>4</v>
+      </c>
+      <c r="N25" t="n">
+        <v>17</v>
+      </c>
+      <c r="O25" t="n">
+        <v>33</v>
+      </c>
+      <c r="P25" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>10</v>
+      </c>
+      <c r="R25" t="n">
+        <v>25</v>
+      </c>
+      <c r="S25" t="n">
+        <v>67</v>
+      </c>
+      <c r="T25" t="n">
+        <v>531</v>
+      </c>
+      <c r="U25" t="n">
+        <v>424</v>
+      </c>
+      <c r="V25" t="n">
+        <v>79.8</v>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="X25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>39</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>13</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>475</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>28</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>16</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>31</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>15</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>69</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>335</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>223</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>66.59999999999999</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Manchester United</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" t="n">
+        <v>25</v>
+      </c>
+      <c r="F26" t="n">
+        <v>5</v>
+      </c>
+      <c r="G26" t="n">
+        <v>62</v>
+      </c>
+      <c r="H26" t="n">
+        <v>9</v>
+      </c>
+      <c r="I26" t="n">
+        <v>7</v>
+      </c>
+      <c r="J26" t="n">
+        <v>26</v>
+      </c>
+      <c r="K26" t="n">
+        <v>674</v>
+      </c>
+      <c r="L26" t="n">
+        <v>16</v>
+      </c>
+      <c r="M26" t="n">
+        <v>3</v>
+      </c>
+      <c r="N26" t="n">
+        <v>21</v>
+      </c>
+      <c r="O26" t="n">
+        <v>20</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>4</v>
+      </c>
+      <c r="R26" t="n">
+        <v>21</v>
+      </c>
+      <c r="S26" t="n">
+        <v>72</v>
+      </c>
+      <c r="T26" t="n">
+        <v>558</v>
+      </c>
+      <c r="U26" t="n">
+        <v>449</v>
+      </c>
+      <c r="V26" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="X26" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>38</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>483</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>38</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>18</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>13</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>77</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>346</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>237</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Leeds United</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" t="n">
+        <v>43</v>
+      </c>
+      <c r="H27" t="n">
+        <v>10</v>
+      </c>
+      <c r="I27" t="n">
+        <v>5</v>
+      </c>
+      <c r="J27" t="n">
+        <v>17</v>
+      </c>
+      <c r="K27" t="n">
+        <v>560</v>
+      </c>
+      <c r="L27" t="n">
+        <v>18</v>
+      </c>
+      <c r="M27" t="n">
+        <v>13</v>
+      </c>
+      <c r="N27" t="n">
+        <v>7</v>
+      </c>
+      <c r="O27" t="n">
+        <v>20</v>
+      </c>
+      <c r="P27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>11</v>
+      </c>
+      <c r="R27" t="n">
+        <v>15</v>
+      </c>
+      <c r="S27" t="n">
+        <v>78</v>
+      </c>
+      <c r="T27" t="n">
+        <v>453</v>
+      </c>
+      <c r="U27" t="n">
+        <v>349</v>
+      </c>
+      <c r="V27" t="n">
+        <v>77</v>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>Newcastle United</t>
+        </is>
+      </c>
+      <c r="X27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>57</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>695</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>7</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>8</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>24</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>79</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>603</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>498</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>82.59999999999999</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Brighton &amp; Hove Albion</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>11</v>
+      </c>
+      <c r="F28" t="n">
+        <v>6</v>
+      </c>
+      <c r="G28" t="n">
+        <v>37</v>
+      </c>
+      <c r="H28" t="n">
+        <v>16</v>
+      </c>
+      <c r="I28" t="n">
+        <v>3</v>
+      </c>
+      <c r="J28" t="n">
+        <v>8</v>
+      </c>
+      <c r="K28" t="n">
+        <v>440</v>
+      </c>
+      <c r="L28" t="n">
+        <v>17</v>
+      </c>
+      <c r="M28" t="n">
+        <v>8</v>
+      </c>
+      <c r="N28" t="n">
+        <v>9</v>
+      </c>
+      <c r="O28" t="n">
+        <v>11</v>
+      </c>
+      <c r="P28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>11</v>
+      </c>
+      <c r="R28" t="n">
+        <v>12</v>
+      </c>
+      <c r="S28" t="n">
+        <v>59</v>
+      </c>
+      <c r="T28" t="n">
+        <v>340</v>
+      </c>
+      <c r="U28" t="n">
+        <v>251</v>
+      </c>
+      <c r="V28" t="n">
+        <v>73.8</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="X28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>63</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>695</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>14</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>15</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>7</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>16</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>48</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>589</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>513</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>87.09999999999999</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Nottingham Forest</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>11</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G29" t="n">
+        <v>58</v>
+      </c>
+      <c r="H29" t="n">
+        <v>14</v>
+      </c>
+      <c r="I29" t="n">
+        <v>9</v>
+      </c>
+      <c r="J29" t="n">
+        <v>35</v>
+      </c>
+      <c r="K29" t="n">
+        <v>707</v>
+      </c>
+      <c r="L29" t="n">
+        <v>19</v>
+      </c>
+      <c r="M29" t="n">
+        <v>6</v>
+      </c>
+      <c r="N29" t="n">
+        <v>12</v>
+      </c>
+      <c r="O29" t="n">
+        <v>17</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>5</v>
+      </c>
+      <c r="R29" t="n">
+        <v>17</v>
+      </c>
+      <c r="S29" t="n">
+        <v>44</v>
+      </c>
+      <c r="T29" t="n">
+        <v>596</v>
+      </c>
+      <c r="U29" t="n">
+        <v>491</v>
+      </c>
+      <c r="V29" t="n">
+        <v>82.40000000000001</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>West Ham United</t>
+        </is>
+      </c>
+      <c r="X29" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>549</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>16</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>36</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>12</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>12</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>51</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>425</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>344</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>80.90000000000001</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" t="n">
+        <v>9</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" t="n">
+        <v>53</v>
+      </c>
+      <c r="H30" t="n">
+        <v>7</v>
+      </c>
+      <c r="I30" t="n">
+        <v>3</v>
+      </c>
+      <c r="J30" t="n">
+        <v>7</v>
+      </c>
+      <c r="K30" t="n">
+        <v>580</v>
+      </c>
+      <c r="L30" t="n">
+        <v>11</v>
+      </c>
+      <c r="M30" t="n">
+        <v>7</v>
+      </c>
+      <c r="N30" t="n">
+        <v>10</v>
+      </c>
+      <c r="O30" t="n">
+        <v>32</v>
+      </c>
+      <c r="P30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>7</v>
+      </c>
+      <c r="R30" t="n">
+        <v>19</v>
+      </c>
+      <c r="S30" t="n">
+        <v>77</v>
+      </c>
+      <c r="T30" t="n">
+        <v>465</v>
+      </c>
+      <c r="U30" t="n">
+        <v>386</v>
+      </c>
+      <c r="V30" t="n">
+        <v>83</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="X30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>47</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>17</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>512</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>20</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>5</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>16</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>69</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>411</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>327</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>79.59999999999999</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Aston Villa</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>13</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4</v>
+      </c>
+      <c r="G31" t="n">
+        <v>59</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7</v>
+      </c>
+      <c r="I31" t="n">
+        <v>10</v>
+      </c>
+      <c r="J31" t="n">
+        <v>31</v>
+      </c>
+      <c r="K31" t="n">
+        <v>681</v>
+      </c>
+      <c r="L31" t="n">
+        <v>11</v>
+      </c>
+      <c r="M31" t="n">
+        <v>6</v>
+      </c>
+      <c r="N31" t="n">
+        <v>6</v>
+      </c>
+      <c r="O31" t="n">
+        <v>16</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>3</v>
+      </c>
+      <c r="R31" t="n">
+        <v>20</v>
+      </c>
+      <c r="S31" t="n">
+        <v>66</v>
+      </c>
+      <c r="T31" t="n">
+        <v>586</v>
+      </c>
+      <c r="U31" t="n">
+        <v>503</v>
+      </c>
+      <c r="V31" t="n">
+        <v>85.8</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="X31" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>41</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>533</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>26</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>9</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>43</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>9</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>50</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>414</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>342</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>82.59999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>